<commit_message>
[DONE] Tractament MF_UF a MF/UF
</commit_message>
<xml_diff>
--- a/public/20220419_SUGGEREIX_Taula_C8.xlsx
+++ b/public/20220419_SUGGEREIX_Taula_C8.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25318"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ficra.sharepoint.com/sites/SADSUGGEREIX/Materiales de clase/Doc_SAD_actualitzada/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="11_AD4D2F04E46CFB4ACB3E2009C513D486683EDF12" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A55E1D9-4F21-42A0-A3DE-AC827E66688E}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="11_AD4D2F04E46CFB4ACB3E2009C513D486683EDF12" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97C12D9D-81EC-4363-879D-313709C4194F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -82,7 +82,7 @@
     <t>FQ_D</t>
   </si>
   <si>
-    <t>Coagulació, floculació</t>
+    <t>Coagulació, floculació i decantació</t>
   </si>
   <si>
     <t>FS</t>
@@ -103,10 +103,10 @@
     <t>Carbó actiu biològic</t>
   </si>
   <si>
-    <t>MF_UF</t>
-  </si>
-  <si>
-    <t>Microfiltració, ultrafiltració</t>
+    <t>MF/UF</t>
+  </si>
+  <si>
+    <t>Microfiltració o ultrafiltració</t>
   </si>
   <si>
     <t>OI</t>
@@ -582,7 +582,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
@@ -793,6 +793,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010042169B78D842A848BE799D251A5B2C6A" ma:contentTypeVersion="7" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="625099e38fc716cc4bb30b36cfa7c837">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="758674b2-73ae-44f0-9f19-d4ad379aa2ea" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c97fa59194b5c482d1d5e2dd6e3e6b4b" ns2:_="">
     <xsd:import namespace="758674b2-73ae-44f0-9f19-d4ad379aa2ea"/>
@@ -956,20 +962,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36B98D60-1B09-41ED-B070-81069043F37F}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5EA6D25-2622-4FBF-8F60-AD25797C2495}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9871CD95-376E-4313-9022-8642DDF9C6B1}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5EA6D25-2622-4FBF-8F60-AD25797C2495}"/>
 </file>
</xml_diff>